<commit_message>
added delete button added more css to cards, fixed login error, fixed edit button showing upp to non logged in users
</commit_message>
<xml_diff>
--- a/testrapport.xlsx
+++ b/testrapport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dat 20\progutv\aspslutuppgift-re\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DE1AD3C-4783-4B58-B2C2-4B03039B903E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADA410B-F620-4660-97C1-2C28A673795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4E2DD77B-7CDB-40CD-A7CF-4C17ABBEC780}"/>
+    <workbookView minimized="1" xWindow="5780" yWindow="4540" windowWidth="7500" windowHeight="6000" xr2:uid="{4E2DD77B-7CDB-40CD-A7CF-4C17ABBEC780}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsivitet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>front page</t>
   </si>
@@ -64,7 +64,70 @@
     <t>780p</t>
   </si>
   <si>
-    <t>1020p</t>
+    <t>create</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>fungerar</t>
+  </si>
+  <si>
+    <t>fungerar inte</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>icke navigerbara filer</t>
+  </si>
+  <si>
+    <t>filtered input</t>
+  </si>
+  <si>
+    <t>fitered output</t>
+  </si>
+  <si>
+    <t>admin level security</t>
+  </si>
+  <si>
+    <t>1080p</t>
+  </si>
+  <si>
+    <t>1920p</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>fungear till en viss del</t>
+  </si>
+  <si>
+    <t>create genre/language/author</t>
+  </si>
+  <si>
+    <t>prepered  functions</t>
+  </si>
+  <si>
+    <t>DOD</t>
+  </si>
+  <si>
+    <t>includes mappen skall inte vara åtkomstbar genom browsern</t>
+  </si>
+  <si>
+    <t>specifika sidor och funktioner skall bara vara tillgängliga åt admins som har loggat in</t>
+  </si>
+  <si>
+    <t>functioner har blivit prepered</t>
   </si>
 </sst>
 </file>
@@ -80,12 +143,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,8 +181,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1080A3B-D599-426C-A9AF-157BB2C7E6AB}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,7 +514,7 @@
     <col min="1" max="1" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -435,37 +522,45 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -475,26 +570,187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF737E5A-74B8-4C79-953E-C2CBBCF118D2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCFDB0C-C309-4B49-B518-DC4605BFB6B1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added comments, fixed css, deleted old garbage code
</commit_message>
<xml_diff>
--- a/testrapport.xlsx
+++ b/testrapport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dat 20\progutv\aspslutuppgift-re\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADA410B-F620-4660-97C1-2C28A673795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89E98666-90E5-47F6-8C8B-8CF99CA55790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5780" yWindow="4540" windowWidth="7500" windowHeight="6000" xr2:uid="{4E2DD77B-7CDB-40CD-A7CF-4C17ABBEC780}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4E2DD77B-7CDB-40CD-A7CF-4C17ABBEC780}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsivitet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>front page</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>functioner har blivit prepered</t>
+  </si>
+  <si>
+    <t>fungerar till viss del</t>
+  </si>
+  <si>
+    <t>admin commands</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +174,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -189,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1080A3B-D599-426C-A9AF-157BB2C7E6AB}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,53 +545,100 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF737E5A-74B8-4C79-953E-C2CBBCF118D2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
     <col min="3" max="3" width="19.6328125" customWidth="1"/>
     <col min="4" max="4" width="11.7265625" customWidth="1"/>
   </cols>
@@ -663,6 +723,16 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>